<commit_message>
CCSB Loads, Outflow, wy2016-18, Sand --- replaced Sand Sigma Plot PDF files and replaced plots for Sand on the Power Points;  Outflow, wy2016-18, pMeHg, fMeHg, wwMeHg: updated Q and WQ worksheet; updated model results; created a second (Part 2) Sigma Plot file, updated the older Sigma Plot file; added new PDF files to the Sigma Plot folder; updated the PowerPoint files; replaced the rloadest folders; updated the Loads Progress Sheet.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Sites/Outflow_11452900/4_wy2016-2018/4_rloadest/4_fMeHg/4_Excel for Text Files/fMeHg_Comb_OutflowR.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Sites/Outflow_11452900/4_wy2016-2018/4_rloadest/4_fMeHg/4_Excel for Text Files/fMeHg_Comb_OutflowR.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Sites\Outflow_11452900\4_wy2016-2018\4_rloadest\4_fMeHg\4_Excel for Text Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCA32853-191F-47DD-9360-C761DE8C460C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E0091B-92F0-48CC-986E-03623BAC00BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61F6959E-92C2-49CE-ACD6-A028EBD9B549}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{61F6959E-92C2-49CE-ACD6-A028EBD9B549}"/>
   </bookViews>
   <sheets>
-    <sheet name="4_fMeHg_Comb" sheetId="1" r:id="rId1"/>
+    <sheet name="4_fMeHg_Comb_31ct" sheetId="1" r:id="rId1"/>
+    <sheet name="4_fMeHg_Comb_30ct" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
   <si>
     <t>Dates</t>
   </si>
@@ -75,12 +76,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -111,12 +118,25 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -430,8 +450,8 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,16 +740,16 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="9">
         <v>42721</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="11">
         <v>0.6</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="12">
         <v>0.09</v>
       </c>
     </row>
@@ -898,6 +918,472 @@
         <v>350</v>
       </c>
       <c r="D33" s="8">
+        <v>0.121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D85F2C3-77F3-4091-A152-1674150AEC9B}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>42389</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C3" s="4">
+        <v>476</v>
+      </c>
+      <c r="D3" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>42392</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C4" s="4">
+        <v>57.7</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>42393</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="C5" s="4">
+        <v>114</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>42402</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C6" s="4">
+        <v>498</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.58368055555555554</v>
+      </c>
+      <c r="C7" s="4">
+        <v>430</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>42404</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C8" s="4">
+        <v>256</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>42436</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="C9" s="4">
+        <v>541</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>42437</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4">
+        <v>551</v>
+      </c>
+      <c r="D10" s="5">
+        <v>7.6999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>42438</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C11" s="4">
+        <v>856</v>
+      </c>
+      <c r="D11" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>42439</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C12" s="4">
+        <v>654</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>42441</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4465</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>42442</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.54895833333333333</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3732</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>42443</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3176</v>
+      </c>
+      <c r="D15" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>42444</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2598</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>42446</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2858</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>42466</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C18" s="4">
+        <v>473</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>42719</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C19" s="4">
+        <v>79.2</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>42720</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C20" s="4">
+        <v>233</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>42744</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="C21" s="4">
+        <v>12332</v>
+      </c>
+      <c r="D21" s="5">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>42745</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C22" s="4">
+        <v>3859</v>
+      </c>
+      <c r="D22" s="5">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>42746</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C23" s="4">
+        <v>13770</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>42767</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3031</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>42774</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.61145833333333333</v>
+      </c>
+      <c r="C25" s="4">
+        <v>10858</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>42776</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C26" s="4">
+        <v>11505</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>42787</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="C27" s="4">
+        <v>13499</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>42810</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.6947916666666667</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2942</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>42829</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C29" s="4">
+        <v>259</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.60451388888888891</v>
+      </c>
+      <c r="C30" s="4">
+        <v>223</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43181</v>
+      </c>
+      <c r="B31" s="7">
+        <v>0.4375</v>
+      </c>
+      <c r="C31">
+        <v>86.2</v>
+      </c>
+      <c r="D31" s="8">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43198</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="C32">
+        <v>350</v>
+      </c>
+      <c r="D32" s="8">
         <v>0.121</v>
       </c>
     </row>

</xml_diff>